<commit_message>
enhance optima script generator
</commit_message>
<xml_diff>
--- a/dbx_context_param_optima.xlsx
+++ b/dbx_context_param_optima.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KLMembrano\OneDrive - PLDT\dbx_automation\dbx_generator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31F5D19-8EAA-4874-8F5A-8AF87FDF8A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BDE74BE-ADA3-4709-B9E3-5F1BCF39C1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="540" activeTab="1" xr2:uid="{15E29264-49B0-4491-96C0-AFEF115122E3}"/>
   </bookViews>
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="186">
   <si>
     <t>iteration</t>
   </si>
@@ -146,9 +146,6 @@
   </si>
   <si>
     <t>p_source_directory</t>
-  </si>
-  <si>
-    <t>p_file_mask</t>
   </si>
   <si>
     <t>mask</t>
@@ -619,55 +616,37 @@
     <t>tenant_id</t>
   </si>
   <si>
-    <t>process_dt</t>
-  </si>
-  <si>
-    <t>dd-MM-yyyy</t>
-  </si>
-  <si>
     <t>load_date</t>
   </si>
   <si>
     <t>current date of when the data was loaded to table</t>
   </si>
   <si>
-    <t>data_source_base_path</t>
-  </si>
-  <si>
-    <t>data_destination_base_path</t>
-  </si>
-  <si>
-    <t>manifest_source_base_path</t>
-  </si>
-  <si>
-    <t>manifest_destination_base_path</t>
-  </si>
-  <si>
-    <t>reprocessing_data_source_base_path</t>
-  </si>
-  <si>
-    <t>reprocessing_data_destination_base_path</t>
-  </si>
-  <si>
-    <t>reprocessing_manifest_source_base_path</t>
-  </si>
-  <si>
-    <t>reprocessing_manifest_destination_base_path</t>
-  </si>
-  <si>
-    <t>optima/raw/databases/full/optima_op_repadmin_db_prd_a/ARBOR/DESCRIPTIONS</t>
-  </si>
-  <si>
-    <t>manifests/source_manifest/optima/raw/databases/full/optima_op_repadmin_db_prd_a/ARBOR/DESCRIPTIONS</t>
-  </si>
-  <si>
-    <t>Unique id of the file</t>
-  </si>
-  <si>
     <t>decimal(10,0)</t>
   </si>
   <si>
     <t>decimal(6,0)</t>
+  </si>
+  <si>
+    <t>/optima/raw/databases/full/optima_op_repadmin_db_prd_a/ARBOR/DESCRIPTIONS/</t>
+  </si>
+  <si>
+    <t>on_prem_p_file_mask</t>
+  </si>
+  <si>
+    <t>s3_source_file_mask</t>
+  </si>
+  <si>
+    <t>s3_manifest_file_mask</t>
+  </si>
+  <si>
+    <t>s3_source_file_dir</t>
+  </si>
+  <si>
+    <t>MANIFESTs*.txt</t>
+  </si>
+  <si>
+    <t>*.parquets</t>
   </si>
 </sst>
 </file>
@@ -1078,12 +1057,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1110,6 +1083,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1678,7 +1655,7 @@
   <dimension ref="A1:K131"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1686,7 +1663,7 @@
     <col min="1" max="1" width="13.59765625" customWidth="1"/>
     <col min="2" max="2" width="20.19921875" customWidth="1"/>
     <col min="3" max="3" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" style="27" customWidth="1"/>
+    <col min="4" max="4" width="15.69921875" style="27" customWidth="1"/>
     <col min="5" max="5" width="11.09765625" customWidth="1"/>
     <col min="9" max="9" width="19.3984375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.59765625" bestFit="1" customWidth="1"/>
@@ -1704,13 +1681,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E1" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="F1" s="38" t="s">
         <v>118</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1719,10 +1696,10 @@
         <v>_c0</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D2" s="28"/>
       <c r="E2" t="str" cm="1">
@@ -1730,13 +1707,13 @@
         <v/>
       </c>
       <c r="I2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -1745,10 +1722,10 @@
         <v>_c1</v>
       </c>
       <c r="B3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D3" s="28"/>
       <c r="E3" t="str" cm="1">
@@ -1763,10 +1740,10 @@
         <v>_c2</v>
       </c>
       <c r="B4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" t="str" cm="1">
@@ -1780,7 +1757,7 @@
         <v>_c3</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -1797,7 +1774,7 @@
         <v>_c4</v>
       </c>
       <c r="B6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -1808,13 +1785,13 @@
         <v/>
       </c>
       <c r="I6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" t="s">
         <v>108</v>
-      </c>
-      <c r="K6" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1823,7 +1800,7 @@
         <v>_c5</v>
       </c>
       <c r="B7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -1834,13 +1811,13 @@
         <v/>
       </c>
       <c r="I7" t="s">
+        <v>106</v>
+      </c>
+      <c r="J7" t="s">
         <v>107</v>
       </c>
-      <c r="J7" t="s">
-        <v>108</v>
-      </c>
       <c r="K7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1849,10 +1826,10 @@
         <v>_c6</v>
       </c>
       <c r="B8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C8" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" t="str" cm="1">
@@ -1860,13 +1837,13 @@
         <v/>
       </c>
       <c r="I8" t="s">
+        <v>158</v>
+      </c>
+      <c r="J8" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" t="s">
         <v>159</v>
-      </c>
-      <c r="J8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1875,7 +1852,7 @@
         <v>_c7</v>
       </c>
       <c r="B9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
@@ -1886,13 +1863,13 @@
         <v/>
       </c>
       <c r="I9" t="s">
+        <v>99</v>
+      </c>
+      <c r="J9" t="s">
         <v>100</v>
       </c>
-      <c r="J9" t="s">
-        <v>101</v>
-      </c>
       <c r="K9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1901,26 +1878,26 @@
         <v>_c8</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D10" t="s">
-        <v>177</v>
+        <v>110</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10">_xlfn.XLOOKUP(B10,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
       </c>
       <c r="I10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J10" t="s">
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -1929,13 +1906,13 @@
         <v>_c9</v>
       </c>
       <c r="B11" t="s">
-        <v>178</v>
+        <v>101</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E11" t="str" cm="1">
         <f t="array" ref="E11">_xlfn.XLOOKUP(B11,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
@@ -1957,42 +1934,34 @@
         <v>_c10</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>101</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>111</v>
+        <v>5</v>
       </c>
       <c r="E12" t="str" cm="1">
         <f t="array" ref="E12">_xlfn.XLOOKUP(B12,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
       </c>
       <c r="I12" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="J12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>IF(B13&lt;&gt;"", "_c" &amp; ROW(B13)-ROW($B$2), "")</f>
-        <v>_c11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" t="s">
-        <v>190</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D13"/>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xlfn.XLOOKUP(B13,TAGS!$A$2:$A$29,TAGS!$B$2:$C$29,"",0)</f>
         <v/>
@@ -2678,18 +2647,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1029" r:id="rId4" name="removeSpace_comma">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="1025" r:id="rId4" name="lowerCase">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>10</xdr:col>
+                <xdr:col>8</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>11</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>1203960</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2698,7 +2667,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1029" r:id="rId4" name="removeSpace_comma"/>
+        <control shapeId="1025" r:id="rId4" name="lowerCase"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2728,18 +2697,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="1025" r:id="rId8" name="lowerCase">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="1029" r:id="rId8" name="removeSpace_comma">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>8</xdr:col>
+                <xdr:col>10</xdr:col>
                 <xdr:colOff>0</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>1203960</xdr:colOff>
+                <xdr:col>11</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -2748,7 +2717,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="1025" r:id="rId8" name="lowerCase"/>
+        <control shapeId="1029" r:id="rId8" name="removeSpace_comma"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -2758,10 +2727,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C60F7B6B-C5E1-4429-85DD-83E208CF5571}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="B3:G28"/>
+  <dimension ref="B3:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2781,24 +2750,24 @@
       <c r="C3" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="45" t="s">
-        <v>152</v>
-      </c>
-      <c r="G3" s="46"/>
+      <c r="F3" s="43" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="44"/>
     </row>
     <row r="4" spans="2:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C4" s="30" t="str">
         <f>IF(C6="silver","_s",IF(C6="bronze","_b",IF(C6="reference"," ","")))</f>
         <v>_b</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
@@ -2806,13 +2775,13 @@
         <v>8</v>
       </c>
       <c r="C5" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
@@ -2820,13 +2789,13 @@
         <v>10</v>
       </c>
       <c r="C6" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="42" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -2834,7 +2803,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="41" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
@@ -2842,13 +2811,13 @@
         <v>11</v>
       </c>
       <c r="C8" s="41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -2856,13 +2825,13 @@
         <v>9</v>
       </c>
       <c r="C9" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -2870,13 +2839,13 @@
         <v>17</v>
       </c>
       <c r="C10" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
@@ -2887,10 +2856,10 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" s="39" t="s">
         <v>149</v>
-      </c>
-      <c r="G11" s="39" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
@@ -2904,7 +2873,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
@@ -2912,23 +2881,23 @@
         <v>19</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>20</v>
+        <v>180</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.3">
@@ -2936,12 +2905,12 @@
         <v>16</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C18" s="32" t="str">
         <f>_xlfn.CONCAT(D18,"_task")</f>
@@ -2954,18 +2923,18 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B19" s="23" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C19" s="32" t="str">
         <f>IF(LOWER(C9)="hourly","txn_date",
-IF(LOWER(C9)="daily","txn_date, load_date",
+IF(LOWER(C9)="daily","txn_date",
 IF(LOWER(C9)="minutes","file_timestamp_bucket, txn_date","")))</f>
-        <v>txn_date, load_date</v>
+        <v>txn_date</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B20" s="34" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C20" s="35" t="str">
         <f>IF(LOWER(C9)="hourly","file_timestamp_bucket",
@@ -2973,68 +2942,28 @@
         <v>txn_date</v>
       </c>
     </row>
-    <row r="21" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="43" t="s">
-        <v>180</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="43" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B22" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="C22" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="43" t="s">
+      <c r="C22" s="32" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B23" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="C23" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="43" t="s">
-        <v>183</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="43" t="s">
+      <c r="C23" s="32" t="s">
         <v>184</v>
-      </c>
-      <c r="C25" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="43" t="s">
-        <v>185</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="43" t="s">
-        <v>186</v>
-      </c>
-      <c r="C27" s="19" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" s="44" customFormat="1" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="43" t="s">
-        <v>187</v>
-      </c>
-      <c r="C28" s="19" t="s">
-        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3064,13 +2993,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="C1" s="37" t="s">
         <v>118</v>
-      </c>
-      <c r="C1" s="37" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3078,307 +3007,307 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
         <v>120</v>
-      </c>
-      <c r="C2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" t="s">
         <v>120</v>
-      </c>
-      <c r="C3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" t="s">
         <v>120</v>
-      </c>
-      <c r="C4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C5" t="s">
         <v>120</v>
-      </c>
-      <c r="C5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" t="s">
         <v>120</v>
-      </c>
-      <c r="C6" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" t="s">
+        <v>119</v>
+      </c>
+      <c r="C7" t="s">
         <v>120</v>
-      </c>
-      <c r="C7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
         <v>120</v>
-      </c>
-      <c r="C8" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" t="s">
         <v>120</v>
-      </c>
-      <c r="C9" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
         <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
         <v>120</v>
-      </c>
-      <c r="C11" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
         <v>120</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" t="s">
         <v>120</v>
-      </c>
-      <c r="C13" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" t="s">
         <v>120</v>
-      </c>
-      <c r="C14" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" t="s">
         <v>120</v>
-      </c>
-      <c r="C15" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" t="s">
         <v>120</v>
-      </c>
-      <c r="C16" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B17" t="s">
+        <v>119</v>
+      </c>
+      <c r="C17" t="s">
         <v>120</v>
-      </c>
-      <c r="C17" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" t="s">
         <v>132</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>133</v>
-      </c>
-      <c r="C18" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
         <v>133</v>
-      </c>
-      <c r="C19" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B20" t="s">
+        <v>132</v>
+      </c>
+      <c r="C20" t="s">
         <v>133</v>
-      </c>
-      <c r="C20" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B21" t="s">
+        <v>132</v>
+      </c>
+      <c r="C21" t="s">
         <v>133</v>
-      </c>
-      <c r="C21" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
         <v>133</v>
-      </c>
-      <c r="C22" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B23" t="s">
+        <v>132</v>
+      </c>
+      <c r="C23" t="s">
         <v>133</v>
-      </c>
-      <c r="C23" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" t="s">
         <v>133</v>
-      </c>
-      <c r="C24" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" t="s">
         <v>133</v>
-      </c>
-      <c r="C25" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
+        <v>132</v>
+      </c>
+      <c r="C26" t="s">
         <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B27" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" t="s">
         <v>133</v>
-      </c>
-      <c r="C27" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B28" t="s">
+        <v>132</v>
+      </c>
+      <c r="C28" t="s">
         <v>133</v>
-      </c>
-      <c r="C28" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B29" t="s">
+        <v>132</v>
+      </c>
+      <c r="C29" t="s">
         <v>133</v>
-      </c>
-      <c r="C29" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -3411,10 +3340,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3564,73 +3493,73 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>8,process_dt</v>
+        <v>8,dbx_process_dttm</v>
       </c>
       <c r="B10" t="str">
         <f>IF(schema!B10&lt;&gt;"", schema!B10, "")</f>
-        <v>process_dt</v>
+        <v>dbx_process_dttm</v>
       </c>
       <c r="C10" t="str">
         <f>IF(schema!C10&lt;&gt;"", schema!C10, "")</f>
-        <v>date</v>
+        <v>timestamp</v>
       </c>
       <c r="D10" s="20" t="str">
         <f>IF(schema!B10&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B10), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B10, 0),"")</f>
-        <v>process_dt</v>
+        <v>dbx_process_dttm</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>9,load_date</v>
+        <v>9,file_name</v>
       </c>
       <c r="B11" t="str">
         <f>IF(schema!B11&lt;&gt;"", schema!B11, "")</f>
-        <v>load_date</v>
+        <v>file_name</v>
       </c>
       <c r="C11" t="str">
         <f>IF(schema!C11&lt;&gt;"", schema!C11, "")</f>
-        <v>date</v>
+        <v>string</v>
       </c>
       <c r="D11" s="20" t="str">
         <f>IF(schema!B11&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B11), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B11, 0),"")</f>
-        <v>load_date</v>
+        <v>file_name</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>10,dbx_process_dttm</v>
+        <v>10,file_id</v>
       </c>
       <c r="B12" t="str">
         <f>IF(schema!B12&lt;&gt;"", schema!B12, "")</f>
-        <v>dbx_process_dttm</v>
+        <v>file_id</v>
       </c>
       <c r="C12" t="str">
         <f>IF(schema!C12&lt;&gt;"", schema!C12, "")</f>
-        <v>timestamp</v>
+        <v>string</v>
       </c>
       <c r="D12" s="20" t="str">
         <f>IF(schema!B12&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B12), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B12, 0),"")</f>
-        <v>dbx_process_dttm</v>
+        <v>file_id</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>11,file_id</v>
+        <v/>
       </c>
       <c r="B13" t="str">
         <f>IF(schema!B13&lt;&gt;"", schema!B13, "")</f>
-        <v>file_id</v>
+        <v/>
       </c>
       <c r="C13" t="str">
         <f>IF(schema!C13&lt;&gt;"", schema!C13, "")</f>
-        <v>string</v>
+        <v/>
       </c>
       <c r="D13" s="20" t="str">
         <f>IF(schema!B13&lt;&gt;"",_xlfn.XLOOKUP(TRIM(B13), masking_fields!$B$2:$B$100, masking_fields!$E$2:$E$100, B13, 0),"")</f>
-        <v>file_id</v>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -6250,22 +6179,22 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
-        <v>23</v>
-      </c>
       <c r="E1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I1" s="1">
         <v>63</v>
@@ -6277,20 +6206,20 @@
         <v>1</v>
       </c>
       <c r="B2" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="20" t="s">
-        <v>25</v>
-      </c>
       <c r="D2" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="20" t="str">
         <f>IF(B2&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B2)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B2), INDEX($I$2:$I$15, MATCH(B2, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(owning_subscriber_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as owning_subscriber_id</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2" s="19" t="str" cm="1">
         <f t="array" ref="I2">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H2)</f>
@@ -6306,10 +6235,10 @@
         <v>3</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="20" t="str">
         <f>IF(B3&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B3)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B3), INDEX($I$2:$I$15, MATCH(B3, $H$2:$H$15, 0))),"")</f>
@@ -6329,20 +6258,20 @@
         <v>3</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="20" t="str">
         <f>IF(B4&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B4)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B4), INDEX($I$2:$I$15, MATCH(B4, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(subscriber_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as subscriber_id</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I4" s="19" t="str" cm="1">
         <f t="array" ref="I4">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H4)</f>
@@ -6355,20 +6284,20 @@
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="20" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>28</v>
       </c>
       <c r="E5" s="20" t="str">
         <f>IF(B5&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B5)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B5), INDEX($I$2:$I$15, MATCH(B5, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(retailer_id), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as retailer_id</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I5" s="19" t="str" cm="1">
         <f t="array" ref="I5">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H5)</f>
@@ -6381,20 +6310,20 @@
         <v>5</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="20" t="str">
         <f>IF(B6&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B6)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B6), INDEX($I$2:$I$15, MATCH(B6, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(ret_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as ret_id</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I6" s="19" t="str" cm="1">
         <f t="array" ref="I6">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H6)</f>
@@ -6407,20 +6336,20 @@
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="20" t="str">
         <f>IF(B7&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B7)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B7), INDEX($I$2:$I$15, MATCH(B7, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(sub_id as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as sub_id</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="19" t="str" cm="1">
         <f t="array" ref="I7">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H7)</f>
@@ -6433,20 +6362,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="20" t="str">
         <f>IF(B8&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B8)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B8), INDEX($I$2:$I$15, MATCH(B8, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(fund_src), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as fund_src</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="19" t="str" cm="1">
         <f t="array" ref="I8">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H8)</f>
@@ -6459,20 +6388,20 @@
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="20" t="str">
         <f>IF(B9&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B9)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B9), INDEX($I$2:$I$15, MATCH(B9, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(imsi), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as imsi</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="19" t="str" cm="1">
         <f t="array" ref="I9">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H9)</f>
@@ -6485,20 +6414,20 @@
         <v>9</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="20" t="str">
         <f>IF(B10&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B10)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B10), INDEX($I$2:$I$15, MATCH(B10, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(callingnumber), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as callingnumber</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I10" s="19" t="str" cm="1">
         <f t="array" ref="I10">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H10)</f>
@@ -6511,20 +6440,20 @@
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="20" t="str">
         <f>IF(B11&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B11)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B11), INDEX($I$2:$I$15, MATCH(B11, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(callednumber), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as callednumber</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I11" s="19" t="str" cm="1">
         <f t="array" ref="I11">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H11)</f>
@@ -6537,20 +6466,20 @@
         <v>11</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="20" t="str">
         <f>IF(B12&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B12)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B12), INDEX($I$2:$I$15, MATCH(B12, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(ret_min as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as ret_min</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I12" s="19" t="str" cm="1">
         <f t="array" ref="I12">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H12)</f>
@@ -6563,20 +6492,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E13" s="20" t="str">
         <f>IF(B13&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B13)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B13), INDEX($I$2:$I$15, MATCH(B13, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(ret_msisdn as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as ret_msisdn</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I13" s="19" t="str" cm="1">
         <f t="array" ref="I13">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H13)</f>
@@ -6589,20 +6518,20 @@
         <v>13</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E14" s="20" t="str">
         <f>IF(B14&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B14)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B14), INDEX($I$2:$I$15, MATCH(B14, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(imei), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as imei</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I14" s="19" t="str" cm="1">
         <f t="array" ref="I14">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H14)</f>
@@ -6615,20 +6544,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E15" s="20" t="str">
         <f>IF(B15&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B15)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B15), INDEX($I$2:$I$15, MATCH(B15, $H$2:$H$15, 0))),"")</f>
         <v>lower(sha2(concat(trim(cast(dsp_min as string)), 'pO7i1cOAu2qQzFcJyaWBMDAShsfhK6uEmNX57h3vK83lPFFqxCHFWhEPzA3pXulQ'),256)) as dsp_min</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="19" t="str" cm="1">
         <f t="array" ref="I15">SUBSTITUTE(_xlfn.IFS($I$1=63,'[1]MASKING-GUIDE'!$I$11,$I$1=9,'[1]MASKING-GUIDE'!$I$8),"&lt;field&gt;",H15)</f>
@@ -6641,13 +6570,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E16" s="20" t="str">
         <f>IF(B16&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B16)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B16), INDEX($I$2:$I$15, MATCH(B16, $H$2:$H$15, 0))),"")</f>
@@ -6660,13 +6589,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E17" s="20" t="str">
         <f>IF(B17&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B17)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B17), INDEX($I$2:$I$15, MATCH(B17, $H$2:$H$15, 0))),"")</f>
@@ -6679,13 +6608,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E18" s="20" t="str">
         <f>IF(B18&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B18)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B18), INDEX($I$2:$I$15, MATCH(B18, $H$2:$H$15, 0))),"")</f>
@@ -6698,13 +6627,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19" s="20" t="str">
         <f>IF(B19&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B19)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B19), INDEX($I$2:$I$15, MATCH(B19, $H$2:$H$15, 0))),"")</f>
@@ -6717,13 +6646,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E20" s="20" t="str">
         <f>IF(B20&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B20)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B20), INDEX($I$2:$I$15, MATCH(B20, $H$2:$H$15, 0))),"")</f>
@@ -6736,13 +6665,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="20" t="str">
         <f>IF(B21&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B21)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B21), INDEX($I$2:$I$15, MATCH(B21, $H$2:$H$15, 0))),"")</f>
@@ -6755,13 +6684,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E22" s="20" t="str">
         <f>IF(B22&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B22)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B22), INDEX($I$2:$I$15, MATCH(B22, $H$2:$H$15, 0))),"")</f>
@@ -6774,13 +6703,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E23" s="20" t="str">
         <f>IF(B23&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B23)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B23), INDEX($I$2:$I$15, MATCH(B23, $H$2:$H$15, 0))),"")</f>
@@ -6793,13 +6722,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E24" s="20" t="str">
         <f>IF(B24&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B24)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B24), INDEX($I$2:$I$15, MATCH(B24, $H$2:$H$15, 0))),"")</f>
@@ -6812,13 +6741,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E25" s="20" t="str">
         <f>IF(B25&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B25)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B25), INDEX($I$2:$I$15, MATCH(B25, $H$2:$H$15, 0))),"")</f>
@@ -6831,13 +6760,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E26" s="20" t="str">
         <f>IF(B26&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B26)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B26), INDEX($I$2:$I$15, MATCH(B26, $H$2:$H$15, 0))),"")</f>
@@ -6850,13 +6779,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E27" s="20" t="str">
         <f>IF(B27&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B27)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B27), INDEX($I$2:$I$15, MATCH(B27, $H$2:$H$15, 0))),"")</f>
@@ -6869,13 +6798,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E28" s="20" t="str">
         <f>IF(B28&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B28)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B28), INDEX($I$2:$I$15, MATCH(B28, $H$2:$H$15, 0))),"")</f>
@@ -6888,13 +6817,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E29" s="20" t="str">
         <f>IF(B29&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B29)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B29), INDEX($I$2:$I$15, MATCH(B29, $H$2:$H$15, 0))),"")</f>
@@ -6907,13 +6836,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E30" s="20" t="str">
         <f>IF(B30&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B30)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B30), INDEX($I$2:$I$15, MATCH(B30, $H$2:$H$15, 0))),"")</f>
@@ -6926,13 +6855,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E31" s="20" t="str">
         <f>IF(B31&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B31)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B31), INDEX($I$2:$I$15, MATCH(B31, $H$2:$H$15, 0))),"")</f>
@@ -6945,13 +6874,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E32" s="20" t="str">
         <f>IF(B32&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B32)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B32), INDEX($I$2:$I$15, MATCH(B32, $H$2:$H$15, 0))),"")</f>
@@ -6964,13 +6893,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E33" s="20" t="str">
         <f>IF(B33&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B33)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B33), INDEX($I$2:$I$15, MATCH(B33, $H$2:$H$15, 0))),"")</f>
@@ -6983,13 +6912,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E34" s="20" t="str">
         <f>IF(B34&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B34)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B34), INDEX($I$2:$I$15, MATCH(B34, $H$2:$H$15, 0))),"")</f>
@@ -7002,13 +6931,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E35" s="20" t="str">
         <f>IF(B35&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B35)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B35), INDEX($I$2:$I$15, MATCH(B35, $H$2:$H$15, 0))),"")</f>
@@ -7024,10 +6953,10 @@
         <v>4</v>
       </c>
       <c r="C36" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D36" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E36" s="20" t="str">
         <f>IF(B36&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B36)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B36), INDEX($I$2:$I$15, MATCH(B36, $H$2:$H$15, 0))),"")</f>
@@ -7040,13 +6969,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E37" s="20" t="str">
         <f>IF(B37&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B37)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B37), INDEX($I$2:$I$15, MATCH(B37, $H$2:$H$15, 0))),"")</f>
@@ -7059,13 +6988,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E38" s="20" t="str">
         <f>IF(B38&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B38)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B38), INDEX($I$2:$I$15, MATCH(B38, $H$2:$H$15, 0))),"")</f>
@@ -7078,13 +7007,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C39" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D39" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E39" s="20" t="str">
         <f>IF(B39&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B39)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B39), INDEX($I$2:$I$15, MATCH(B39, $H$2:$H$15, 0))),"")</f>
@@ -7097,13 +7026,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D40" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E40" s="20" t="str">
         <f>IF(B40&lt;&gt;"",IF(COUNTIF($H$2:$H$15,B40)=0, SUBSTITUTE('MASKING-GUIDE'!$I$20,"&lt;field&gt;",B40), INDEX($I$2:$I$15, MATCH(B40, $H$2:$H$15, 0))),"")</f>
@@ -7566,7 +7495,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -7594,7 +7523,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -7637,13 +7566,13 @@
       <c r="F7" s="8"/>
       <c r="G7" s="4"/>
       <c r="H7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="K7" s="12"/>
     </row>
@@ -7652,20 +7581,20 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="50" t="s">
+      <c r="E8" s="48" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="50" t="s">
+      <c r="G8" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="G8" s="11" t="s">
+      <c r="H8" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="I8" s="13" t="s">
         <v>69</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>70</v>
       </c>
       <c r="J8" s="14"/>
       <c r="K8" s="12"/>
@@ -7675,16 +7604,16 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
       <c r="G9" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>72</v>
-      </c>
       <c r="I9" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J9" s="14" t="b">
         <v>1</v>
@@ -7709,20 +7638,20 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="50" t="s">
+      <c r="E11" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="50" t="s">
+      <c r="G11" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>76</v>
       </c>
       <c r="J11" s="14"/>
       <c r="K11" s="12"/>
@@ -7732,16 +7661,16 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
       <c r="G12" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>72</v>
-      </c>
       <c r="I12" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J12" s="14" t="b">
         <v>1</v>
@@ -7769,7 +7698,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H14" s="4">
         <v>64</v>
@@ -7800,7 +7729,7 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
@@ -7843,13 +7772,13 @@
       <c r="F19" s="8"/>
       <c r="G19" s="4"/>
       <c r="H19" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="J19" s="11" t="s">
         <v>64</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>65</v>
       </c>
       <c r="K19" s="4"/>
     </row>
@@ -7858,20 +7787,20 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="52" t="s">
+      <c r="G20" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="13" t="s">
+      <c r="I20" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="I20" s="13" t="s">
-        <v>82</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="4"/>
@@ -7881,16 +7810,16 @@
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="53"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="51"/>
       <c r="G21" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J21" s="14" t="b">
         <v>1</v>
@@ -7928,14 +7857,14 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="47" t="s">
-        <v>84</v>
-      </c>
-      <c r="F24" s="48"/>
-      <c r="G24" s="48"/>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="49"/>
+      <c r="E24" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="47"/>
       <c r="K24" s="4"/>
     </row>
   </sheetData>

</xml_diff>